<commit_message>
checkin with static template
</commit_message>
<xml_diff>
--- a/excelgen/src/main/resources/person_template.xlsx
+++ b/excelgen/src/main/resources/person_template.xlsx
@@ -11,22 +11,49 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A6" authorId="0">
+      <text>
+        <t>JXLS Command:
+This row contains the jx:if condition.
+If condition is true, the next row(s) will be included.
+If false, they will be removed from output.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Person Report</t>
   </si>
   <si>
-    <t>Name: ${person.name}</t>
+    <t>Name:</t>
   </si>
   <si>
-    <t>Age: ${person.age}</t>
+    <t>${person.name}</t>
   </si>
   <si>
-    <t>jx:if(condition="person.age &lt; 18" lastCell="A5" areas=["A5:A5"])</t>
+    <t>Age:</t>
   </si>
   <si>
-    <t>Parent: ${person.parentName}</t>
+    <t>${person.age}</t>
+  </si>
+  <si>
+    <t>jx:if(condition="person.age &lt; 18", lastCell="B6")</t>
+  </si>
+  <si>
+    <t>Parent:</t>
+  </si>
+  <si>
+    <t>${person.parentName}</t>
   </si>
 </sst>
 </file>
@@ -57,12 +84,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor indexed="22"/>
+        <fgColor indexed="43"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="22"/>
+        <fgColor indexed="43"/>
       </patternFill>
     </fill>
   </fills>
@@ -86,15 +113,20 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="31.25" customWidth="true"/>
+    <col min="1" max="1" width="15.625" customWidth="true"/>
+    <col min="2" max="2" width="23.4375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -107,23 +139,35 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>3</v>
+    <row r="5"/>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>5</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>4</v>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>